<commit_message>
design system test for regulus
</commit_message>
<xml_diff>
--- a/regulus/test/system_spec.xlsx
+++ b/regulus/test/system_spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>テスト項目</t>
     <rPh sb="3" eb="5">
@@ -48,31 +48,164 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>グラフが表示されている</t>
+    <t>Webページにアクセス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Query</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Path</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.0.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>通貨情報更新</t>
+    <rPh sb="0" eb="4">
+      <t>ツウカジョウホウ</t>
+    </rPh>
     <rPh sb="4" eb="6">
-      <t>ヒョウジ</t>
+      <t>コウシン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Webページにアクセス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Webページにアクセス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>情報(ツイート・日経記事)が表示されている</t>
-    <rPh sb="0" eb="2">
-      <t>ジョウホウ</t>
+    <t>/update_currency</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ツイート更新</t>
+    <rPh sb="4" eb="6">
+      <t>コウシン</t>
     </rPh>
-    <rPh sb="8" eb="12">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/update_tweet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日経記事更新</t>
+    <rPh sb="0" eb="4">
       <t>ニッケイキジ</t>
     </rPh>
-    <rPh sb="14" eb="16">
-      <t>ヒョウジ</t>
+    <rPh sb="4" eb="6">
+      <t>コウシン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/update_article</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>currencies_usd: [&lt;USDJPYの通貨情報&gt;]
+currencies_eur: [&lt;EURJPYの通貨情報&gt;]
+currencies_gbp: [&lt;GBPJPYの通貨情報&gt;]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: ok
+currencies_usd: [&lt;USDJPYの通貨情報&gt;]
+currencies_eur: [&lt;EURJPYの通貨情報&gt;]
+currencies_gbp: [&lt;GBPJPYの通貨情報&gt;]
+tweets: [&lt;ツイート&gt;]
+articles: [&lt;記事&gt;]</t>
+    <rPh sb="36" eb="40">
+      <t>ツウカジョウホウ</t>
+    </rPh>
+    <rPh sb="68" eb="72">
+      <t>ツウカジョウホウ</t>
+    </rPh>
+    <rPh sb="100" eb="104">
+      <t>ツウカジョウホウ</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>キジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tweets: [&lt;ツイート&gt;]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>articles: [&lt;記事&gt;]</t>
+    <rPh sb="12" eb="14">
+      <t>キジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Webページにアクセス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Controller</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>View</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>View</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;div id="currency"&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;div id="tweet"&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;div id="article"&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -129,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -307,6 +440,167 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -317,7 +611,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -335,6 +629,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -668,19 +1019,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E4"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="5" width="70.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="8" width="40.1640625" customWidth="1"/>
+    <col min="9" max="9" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="19" thickBot="1"/>
-    <row r="2" spans="2:5" ht="19" thickBot="1">
+    <row r="1" spans="2:9" ht="19" thickBot="1"/>
+    <row r="2" spans="2:9" ht="19" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -690,36 +1046,202 @@
       <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="4">
+    <row r="3" spans="2:9" ht="83">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="44">
+      <c r="B4" s="24">
+        <v>2</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="29">
+        <v>3</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="24">
+        <v>4</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="29">
+        <v>5</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="29">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>5</v>
+      <c r="C8" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="19" thickBot="1">
-      <c r="B4" s="9">
-        <v>2</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="11" t="s">
+    <row r="9" spans="2:9" ht="19" thickBot="1">
+      <c r="B9" s="20">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>8</v>
+      <c r="C9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -736,19 +1258,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E4"/>
+  <dimension ref="B1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="5" width="70.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="8" width="40.1640625" customWidth="1"/>
+    <col min="9" max="9" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="19" thickBot="1"/>
-    <row r="2" spans="2:5" ht="19" thickBot="1">
+    <row r="1" spans="2:9" ht="19" thickBot="1"/>
+    <row r="2" spans="2:9" ht="19" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -758,25 +1285,43 @@
       <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:9">
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="2:5" ht="19" thickBot="1">
+    <row r="4" spans="2:9" ht="19" thickBot="1">
       <c r="B4" s="9">
         <v>2</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
modify test spec for regulus
</commit_message>
<xml_diff>
--- a/regulus/test/system_spec.xlsx
+++ b/regulus/test/system_spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -94,18 +94,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/update_currency</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ツイート更新</t>
     <rPh sb="4" eb="6">
       <t>コウシン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/update_tweet</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -123,34 +115,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/update_article</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>currencies_usd: [&lt;USDJPYの通貨情報&gt;]
 currencies_eur: [&lt;EURJPYの通貨情報&gt;]
 currencies_gbp: [&lt;GBPJPYの通貨情報&gt;]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: ok
-currencies_usd: [&lt;USDJPYの通貨情報&gt;]
-currencies_eur: [&lt;EURJPYの通貨情報&gt;]
-currencies_gbp: [&lt;GBPJPYの通貨情報&gt;]
-tweets: [&lt;ツイート&gt;]
-articles: [&lt;記事&gt;]</t>
-    <rPh sb="36" eb="40">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="68" eb="72">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="100" eb="104">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="136" eb="138">
-      <t>キジ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -206,6 +173,22 @@
   </si>
   <si>
     <t>&lt;div id="article"&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/tweet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/article</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/currency</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: ok</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1022,7 +1005,7 @@
   <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1047,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>6</v>
@@ -1062,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="83">
+    <row r="3" spans="2:9">
       <c r="B3" s="16">
         <v>1</v>
       </c>
@@ -1073,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>10</v>
@@ -1085,7 +1068,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="44">
@@ -1099,10 +1082,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G4" s="27" t="s">
         <v>11</v>
@@ -1111,7 +1094,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -1122,22 +1105,22 @@
         <v>13</v>
       </c>
       <c r="D5" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>18</v>
       </c>
       <c r="H5" s="32" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -1148,13 +1131,13 @@
         <v>13</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G6" s="27" t="s">
         <v>11</v>
@@ -1163,7 +1146,7 @@
         <v>11</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -1174,13 +1157,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G7" s="32" t="s">
         <v>11</v>
@@ -1189,7 +1172,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="33" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -1200,22 +1183,22 @@
         <v>13</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="19" thickBot="1">
@@ -1226,22 +1209,22 @@
         <v>13</v>
       </c>
       <c r="D9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="22" t="s">
+      <c r="H9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>31</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>